<commit_message>
Added In RP4 Graphs
</commit_message>
<xml_diff>
--- a/Results Summary RPi4.xlsx
+++ b/Results Summary RPi4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5CC96F-BDCE-43EE-93B7-E6AF41920E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F923912-44FB-493A-B67F-B790259D6633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,6 +353,72 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>294674</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>169398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C491BDE-9F8C-343D-BAEB-D7705523C931}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8771924" y="1390650"/>
+          <a:ext cx="8820751" cy="5446248"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -653,7 +719,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4030,5 +4096,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated RPi4 NN Data
</commit_message>
<xml_diff>
--- a/Results Summary RPi4.xlsx
+++ b/Results Summary RPi4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajayv\Documents\projects\UNI\22WSD530-Programming-Multi-many-core-Systems-Coursework-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319114F3-A7B6-42F2-ABCA-0B8A1976FDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05A690E-38D9-4D36-B9BE-6812F3FB58CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,22 +358,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>11907</xdr:rowOff>
+      <xdr:colOff>193676</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>142877</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7F5BECE-6B08-9C5D-9524-10A8608AFB27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0DA7FE-480C-AD8F-AC1E-EBA18FB84130}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -395,8 +395,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8648699" y="1345407"/>
-          <a:ext cx="9715501" cy="5464970"/>
+          <a:off x="8670926" y="1323975"/>
+          <a:ext cx="10007599" cy="5629275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,7 +708,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,13 +790,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
-        <v>2757400</v>
+        <v>2438672</v>
       </c>
       <c r="B3" s="14">
-        <v>3641194</v>
+        <v>3801071</v>
       </c>
       <c r="C3" s="15">
-        <v>38779311</v>
+        <v>38323776</v>
       </c>
       <c r="D3" s="13">
         <v>5948061</v>
@@ -824,34 +824,34 @@
       </c>
       <c r="N3" s="1">
         <f>SUM(A$3:A$102)/100</f>
-        <v>2934446.64</v>
+        <v>2906273.21</v>
       </c>
       <c r="O3" s="2">
         <f>SUM(B$3:B$102)/100</f>
-        <v>3607304.42</v>
+        <v>3562456.84</v>
       </c>
       <c r="P3" s="3">
         <f>SUM(C$3:C$102)/100</f>
-        <v>39797045.75</v>
+        <v>40408552.969999999</v>
       </c>
       <c r="Q3" s="1">
         <f>N3/O3</f>
-        <v>0.81347352436642983</v>
+        <v>0.81580587233163504</v>
       </c>
       <c r="R3" s="3">
         <f>N3/P3</f>
-        <v>7.373528825314879E-2</v>
+        <v>7.1922229240865596E-2</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <v>4067554</v>
+        <v>2973106</v>
       </c>
       <c r="B4" s="17">
-        <v>3573473</v>
+        <v>3353283</v>
       </c>
       <c r="C4" s="18">
-        <v>38068142</v>
+        <v>39362460</v>
       </c>
       <c r="D4" s="16">
         <v>6355293</v>
@@ -900,13 +900,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <v>2287873</v>
+        <v>2836850</v>
       </c>
       <c r="B5" s="17">
-        <v>3688378</v>
+        <v>3814552</v>
       </c>
       <c r="C5" s="18">
-        <v>39578627</v>
+        <v>41096683</v>
       </c>
       <c r="D5" s="16">
         <v>3542000</v>
@@ -953,13 +953,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>3946557</v>
+        <v>2751925</v>
       </c>
       <c r="B6" s="17">
-        <v>5247491</v>
+        <v>3179417</v>
       </c>
       <c r="C6" s="18">
-        <v>37866536</v>
+        <v>41929444</v>
       </c>
       <c r="D6" s="16">
         <v>6758563</v>
@@ -1006,13 +1006,13 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
-        <v>2811602</v>
+        <v>2602298</v>
       </c>
       <c r="B7" s="17">
-        <v>3021356</v>
+        <v>2987032</v>
       </c>
       <c r="C7" s="18">
-        <v>39955266</v>
+        <v>40764079</v>
       </c>
       <c r="D7" s="16">
         <v>3511167</v>
@@ -1038,13 +1038,13 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>3587640</v>
+        <v>3883791</v>
       </c>
       <c r="B8" s="17">
-        <v>4363658</v>
+        <v>3309489</v>
       </c>
       <c r="C8" s="18">
-        <v>40408607</v>
+        <v>39350663</v>
       </c>
       <c r="D8" s="16">
         <v>3920196</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>2561829</v>
+        <v>2986957</v>
       </c>
       <c r="B9" s="17">
-        <v>3317498</v>
+        <v>4018770</v>
       </c>
       <c r="C9" s="18">
-        <v>35463462</v>
+        <v>39569344</v>
       </c>
       <c r="D9" s="16">
         <v>3935900</v>
@@ -1102,13 +1102,13 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <v>2389908</v>
+        <v>3336709</v>
       </c>
       <c r="B10" s="17">
-        <v>4019334</v>
+        <v>3014328</v>
       </c>
       <c r="C10" s="18">
-        <v>38161548</v>
+        <v>39776432</v>
       </c>
       <c r="D10" s="16">
         <v>3995954</v>
@@ -1134,13 +1134,13 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
-        <v>2738900</v>
+        <v>2430728</v>
       </c>
       <c r="B11" s="17">
-        <v>4502341</v>
+        <v>3061789</v>
       </c>
       <c r="C11" s="18">
-        <v>38558761</v>
+        <v>42074163</v>
       </c>
       <c r="D11" s="16">
         <v>3523112</v>
@@ -1166,13 +1166,13 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
-        <v>4010056</v>
+        <v>4438168</v>
       </c>
       <c r="B12" s="17">
-        <v>3270610</v>
+        <v>3600112</v>
       </c>
       <c r="C12" s="18">
-        <v>43196117</v>
+        <v>40600341</v>
       </c>
       <c r="D12" s="16">
         <v>3947492</v>
@@ -1198,13 +1198,13 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
-        <v>3333460</v>
+        <v>2922293</v>
       </c>
       <c r="B13" s="17">
-        <v>3729322</v>
+        <v>4348448</v>
       </c>
       <c r="C13" s="18">
-        <v>39379427</v>
+        <v>44263304</v>
       </c>
       <c r="D13" s="16">
         <v>5943099</v>
@@ -1230,13 +1230,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
-        <v>3141761</v>
+        <v>2777740</v>
       </c>
       <c r="B14" s="17">
-        <v>4455213</v>
+        <v>3209749</v>
       </c>
       <c r="C14" s="18">
-        <v>34304267</v>
+        <v>42047812</v>
       </c>
       <c r="D14" s="16">
         <v>3849179</v>
@@ -1262,13 +1262,13 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
-        <v>3242869</v>
+        <v>3064030</v>
       </c>
       <c r="B15" s="17">
-        <v>4788797</v>
+        <v>3333303</v>
       </c>
       <c r="C15" s="18">
-        <v>35632050</v>
+        <v>40278625</v>
       </c>
       <c r="D15" s="16">
         <v>6440495</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
-        <v>2419852</v>
+        <v>2979606</v>
       </c>
       <c r="B16" s="17">
-        <v>3104558</v>
+        <v>3431745</v>
       </c>
       <c r="C16" s="18">
-        <v>39250894</v>
+        <v>33334600</v>
       </c>
       <c r="D16" s="16">
         <v>3547333</v>
@@ -1326,13 +1326,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
-        <v>3316109</v>
+        <v>2291064</v>
       </c>
       <c r="B17" s="17">
-        <v>5655037</v>
+        <v>2991921</v>
       </c>
       <c r="C17" s="18">
-        <v>39604126</v>
+        <v>40254385</v>
       </c>
       <c r="D17" s="16">
         <v>3991751</v>
@@ -1358,13 +1358,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
-        <v>3075429</v>
+        <v>2415636</v>
       </c>
       <c r="B18" s="17">
-        <v>3224519</v>
+        <v>2617668</v>
       </c>
       <c r="C18" s="18">
-        <v>36694916</v>
+        <v>42175458</v>
       </c>
       <c r="D18" s="16">
         <v>3876049</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
-        <v>4232291</v>
+        <v>2540170</v>
       </c>
       <c r="B19" s="17">
-        <v>3156205</v>
+        <v>2809147</v>
       </c>
       <c r="C19" s="18">
-        <v>36303536</v>
+        <v>39120427</v>
       </c>
       <c r="D19" s="16">
         <v>3487002</v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
-        <v>2295133</v>
+        <v>2947051</v>
       </c>
       <c r="B20" s="17">
-        <v>3337775</v>
+        <v>4548278</v>
       </c>
       <c r="C20" s="18">
-        <v>39634182</v>
+        <v>39991595</v>
       </c>
       <c r="D20" s="16">
         <v>4380149</v>
@@ -1454,13 +1454,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
-        <v>3562121</v>
+        <v>2571559</v>
       </c>
       <c r="B21" s="17">
-        <v>3544381</v>
+        <v>3578575</v>
       </c>
       <c r="C21" s="18">
-        <v>41493972</v>
+        <v>38207168</v>
       </c>
       <c r="D21" s="16">
         <v>5879952</v>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
-        <v>2991617</v>
+        <v>2615132</v>
       </c>
       <c r="B22" s="17">
-        <v>4700207</v>
+        <v>4168322</v>
       </c>
       <c r="C22" s="18">
-        <v>40724008</v>
+        <v>39024392</v>
       </c>
       <c r="D22" s="16">
         <v>3540056</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
-        <v>2297373</v>
+        <v>2797128</v>
       </c>
       <c r="B23" s="17">
-        <v>3222111</v>
+        <v>2991346</v>
       </c>
       <c r="C23" s="18">
-        <v>39568646</v>
+        <v>39926540</v>
       </c>
       <c r="D23" s="16">
         <v>6218389</v>
@@ -1550,13 +1550,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
-        <v>4478600</v>
+        <v>3362098</v>
       </c>
       <c r="B24" s="17">
-        <v>3575344</v>
+        <v>3006661</v>
       </c>
       <c r="C24" s="18">
-        <v>39511740</v>
+        <v>41971943</v>
       </c>
       <c r="D24" s="16">
         <v>5531551</v>
@@ -1582,13 +1582,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
-        <v>2871304</v>
+        <v>2553966</v>
       </c>
       <c r="B25" s="17">
-        <v>3326479</v>
+        <v>5537053</v>
       </c>
       <c r="C25" s="18">
-        <v>45445548</v>
+        <v>39116557</v>
       </c>
       <c r="D25" s="16">
         <v>3779106</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
-        <v>4405232</v>
+        <v>2556762</v>
       </c>
       <c r="B26" s="17">
-        <v>3535345</v>
+        <v>3656944</v>
       </c>
       <c r="C26" s="18">
-        <v>41775966</v>
+        <v>39636827</v>
       </c>
       <c r="D26" s="16">
         <v>5114283</v>
@@ -1646,13 +1646,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
-        <v>2288225</v>
+        <v>3817255</v>
       </c>
       <c r="B27" s="17">
-        <v>3648305</v>
+        <v>4300579</v>
       </c>
       <c r="C27" s="18">
-        <v>44244058</v>
+        <v>40973170</v>
       </c>
       <c r="D27" s="16">
         <v>4043434</v>
@@ -1678,13 +1678,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
-        <v>4048647</v>
+        <v>2596299</v>
       </c>
       <c r="B28" s="17">
-        <v>3312276</v>
+        <v>4271876</v>
       </c>
       <c r="C28" s="18">
-        <v>38785961</v>
+        <v>40511197</v>
       </c>
       <c r="D28" s="16">
         <v>5670678</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>3072910</v>
+        <v>2579392</v>
       </c>
       <c r="B29" s="17">
-        <v>3925965</v>
+        <v>2964199</v>
       </c>
       <c r="C29" s="18">
-        <v>38388969</v>
+        <v>38717938</v>
       </c>
       <c r="D29" s="16">
         <v>3783718</v>
@@ -1742,13 +1742,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
-        <v>2793769</v>
+        <v>2564967</v>
       </c>
       <c r="B30" s="17">
-        <v>3202778</v>
+        <v>4204562</v>
       </c>
       <c r="C30" s="18">
-        <v>39399502</v>
+        <v>39070819</v>
       </c>
       <c r="D30" s="16">
         <v>4806419</v>
@@ -1774,13 +1774,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
-        <v>3856726</v>
+        <v>3595482</v>
       </c>
       <c r="B31" s="17">
-        <v>3622343</v>
+        <v>3306174</v>
       </c>
       <c r="C31" s="18">
-        <v>40486033</v>
+        <v>40773674</v>
       </c>
       <c r="D31" s="16">
         <v>4571535</v>
@@ -1806,13 +1806,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>3014893</v>
+        <v>3823847</v>
       </c>
       <c r="B32" s="17">
-        <v>3815986</v>
+        <v>3299174</v>
       </c>
       <c r="C32" s="18">
-        <v>38026386</v>
+        <v>40762414</v>
       </c>
       <c r="D32" s="16">
         <v>4121970</v>
@@ -1838,13 +1838,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
-        <v>2181265</v>
+        <v>2236436</v>
       </c>
       <c r="B33" s="17">
-        <v>4817963</v>
+        <v>3445892</v>
       </c>
       <c r="C33" s="18">
-        <v>39994210</v>
+        <v>41250553</v>
       </c>
       <c r="D33" s="16">
         <v>5852360</v>
@@ -1870,13 +1870,13 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
-        <v>2547848</v>
+        <v>3271267</v>
       </c>
       <c r="B34" s="17">
-        <v>4302457</v>
+        <v>3487429</v>
       </c>
       <c r="C34" s="18">
-        <v>41859353</v>
+        <v>38254780</v>
       </c>
       <c r="D34" s="16">
         <v>5463998</v>
@@ -1902,13 +1902,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="16">
-        <v>2488795</v>
+        <v>2775851</v>
       </c>
       <c r="B35" s="17">
-        <v>3848967</v>
+        <v>2748481</v>
       </c>
       <c r="C35" s="18">
-        <v>38069514</v>
+        <v>41912207</v>
       </c>
       <c r="D35" s="16">
         <v>3555056</v>
@@ -1934,13 +1934,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="16">
-        <v>2379705</v>
+        <v>3323598</v>
       </c>
       <c r="B36" s="17">
-        <v>4617393</v>
+        <v>3246063</v>
       </c>
       <c r="C36" s="18">
-        <v>42540522</v>
+        <v>39712936</v>
       </c>
       <c r="D36" s="16">
         <v>3945826</v>
@@ -1966,13 +1966,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
-        <v>2530405</v>
+        <v>2393451</v>
       </c>
       <c r="B37" s="17">
-        <v>4710818</v>
+        <v>3583686</v>
       </c>
       <c r="C37" s="18">
-        <v>39293727</v>
+        <v>38731400</v>
       </c>
       <c r="D37" s="16">
         <v>3843272</v>
@@ -1998,13 +1998,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="16">
-        <v>3204945</v>
+        <v>2418765</v>
       </c>
       <c r="B38" s="17">
-        <v>3606288</v>
+        <v>2927126</v>
       </c>
       <c r="C38" s="18">
-        <v>39763604</v>
+        <v>38777270</v>
       </c>
       <c r="D38" s="16">
         <v>6376737</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="16">
-        <v>2703586</v>
+        <v>2251657</v>
       </c>
       <c r="B39" s="17">
-        <v>3400514</v>
+        <v>2760889</v>
       </c>
       <c r="C39" s="18">
-        <v>43056955</v>
+        <v>39913339</v>
       </c>
       <c r="D39" s="16">
         <v>4252227</v>
@@ -2062,13 +2062,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
-        <v>4034222</v>
+        <v>2390525</v>
       </c>
       <c r="B40" s="17">
-        <v>3559529</v>
+        <v>3621389</v>
       </c>
       <c r="C40" s="18">
-        <v>42310472</v>
+        <v>40928763</v>
       </c>
       <c r="D40" s="16">
         <v>5789380</v>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="16">
-        <v>2912099</v>
+        <v>2426913</v>
       </c>
       <c r="B41" s="17">
-        <v>3039300</v>
+        <v>3410245</v>
       </c>
       <c r="C41" s="18">
-        <v>41362365</v>
+        <v>40943059</v>
       </c>
       <c r="D41" s="16">
         <v>3802754</v>
@@ -2126,13 +2126,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
-        <v>2379871</v>
+        <v>2751573</v>
       </c>
       <c r="B42" s="17">
-        <v>3360181</v>
+        <v>3925438</v>
       </c>
       <c r="C42" s="18">
-        <v>39300376</v>
+        <v>43986553</v>
       </c>
       <c r="D42" s="16">
         <v>3926326</v>
@@ -2158,13 +2158,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="16">
-        <v>2539052</v>
+        <v>2858145</v>
       </c>
       <c r="B43" s="17">
-        <v>3249777</v>
+        <v>3289025</v>
       </c>
       <c r="C43" s="18">
-        <v>39294746</v>
+        <v>39728694</v>
       </c>
       <c r="D43" s="16">
         <v>3715867</v>
@@ -2190,13 +2190,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
-        <v>2549553</v>
+        <v>3010475</v>
       </c>
       <c r="B44" s="17">
-        <v>3177612</v>
+        <v>3053475</v>
       </c>
       <c r="C44" s="18">
-        <v>40486719</v>
+        <v>39055597</v>
       </c>
       <c r="D44" s="16">
         <v>3834124</v>
@@ -2222,13 +2222,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
-        <v>2616884</v>
+        <v>3269859</v>
       </c>
       <c r="B45" s="17">
-        <v>3364367</v>
+        <v>3410634</v>
       </c>
       <c r="C45" s="18">
-        <v>39055418</v>
+        <v>39639104</v>
       </c>
       <c r="D45" s="16">
         <v>3964436</v>
@@ -2254,13 +2254,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
-        <v>4215403</v>
+        <v>2429747</v>
       </c>
       <c r="B46" s="17">
-        <v>3512104</v>
+        <v>4449057</v>
       </c>
       <c r="C46" s="18">
-        <v>40600772</v>
+        <v>42998813</v>
       </c>
       <c r="D46" s="16">
         <v>4412741</v>
@@ -2286,13 +2286,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="16">
-        <v>3355886</v>
+        <v>2546930</v>
       </c>
       <c r="B47" s="17">
-        <v>3442254</v>
+        <v>3360191</v>
       </c>
       <c r="C47" s="18">
-        <v>42019147</v>
+        <v>40385459</v>
       </c>
       <c r="D47" s="16">
         <v>6415126</v>
@@ -2318,13 +2318,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
-        <v>3001116</v>
+        <v>3881180</v>
       </c>
       <c r="B48" s="17">
-        <v>3877485</v>
+        <v>3588538</v>
       </c>
       <c r="C48" s="18">
-        <v>42013943</v>
+        <v>40179446</v>
       </c>
       <c r="D48" s="16">
         <v>3436132</v>
@@ -2350,13 +2350,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
-        <v>2471813</v>
+        <v>2639928</v>
       </c>
       <c r="B49" s="17">
-        <v>4068073</v>
+        <v>6849119</v>
       </c>
       <c r="C49" s="18">
-        <v>40226948</v>
+        <v>40368333</v>
       </c>
       <c r="D49" s="16">
         <v>6573159</v>
@@ -2382,13 +2382,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="16">
-        <v>4040759</v>
+        <v>3736960</v>
       </c>
       <c r="B50" s="17">
-        <v>3628805</v>
+        <v>3679480</v>
       </c>
       <c r="C50" s="18">
-        <v>38760111</v>
+        <v>40496552</v>
       </c>
       <c r="D50" s="16">
         <v>3869605</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="16">
-        <v>2574719</v>
+        <v>3154880</v>
       </c>
       <c r="B51" s="17">
-        <v>3794654</v>
+        <v>3564631</v>
       </c>
       <c r="C51" s="18">
-        <v>41119001</v>
+        <v>38751365</v>
       </c>
       <c r="D51" s="16">
         <v>3685478</v>
@@ -2446,13 +2446,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="16">
-        <v>4129831</v>
+        <v>3874420</v>
       </c>
       <c r="B52" s="17">
-        <v>3333071</v>
+        <v>4484261</v>
       </c>
       <c r="C52" s="18">
-        <v>40956838</v>
+        <v>40962783</v>
       </c>
       <c r="D52" s="16">
         <v>3448095</v>
@@ -2478,13 +2478,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
-        <v>2894933</v>
+        <v>2386470</v>
       </c>
       <c r="B53" s="17">
-        <v>3379014</v>
+        <v>2588670</v>
       </c>
       <c r="C53" s="18">
-        <v>42600411</v>
+        <v>40977875</v>
       </c>
       <c r="D53" s="16">
         <v>3937215</v>
@@ -2510,13 +2510,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
-        <v>3679212</v>
+        <v>3908717</v>
       </c>
       <c r="B54" s="17">
-        <v>3279017</v>
+        <v>2788665</v>
       </c>
       <c r="C54" s="18">
-        <v>39415521</v>
+        <v>37359560</v>
       </c>
       <c r="D54" s="16">
         <v>3945918</v>
@@ -2542,13 +2542,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
-        <v>2475998</v>
+        <v>2936792</v>
       </c>
       <c r="B55" s="17">
-        <v>3075484</v>
+        <v>2945218</v>
       </c>
       <c r="C55" s="18">
-        <v>40350889</v>
+        <v>41727860</v>
       </c>
       <c r="D55" s="16">
         <v>3926548</v>
@@ -2574,13 +2574,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="16">
-        <v>3212593</v>
+        <v>2713204</v>
       </c>
       <c r="B56" s="17">
-        <v>4443212</v>
+        <v>5003324</v>
       </c>
       <c r="C56" s="18">
-        <v>40692159</v>
+        <v>40800397</v>
       </c>
       <c r="D56" s="16">
         <v>3907993</v>
@@ -2606,13 +2606,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="16">
-        <v>3387107</v>
+        <v>2583855</v>
       </c>
       <c r="B57" s="17">
-        <v>3066689</v>
+        <v>3444207</v>
       </c>
       <c r="C57" s="18">
-        <v>41394809</v>
+        <v>39609144</v>
       </c>
       <c r="D57" s="16">
         <v>3914808</v>
@@ -2638,13 +2638,13 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="16">
-        <v>2478554</v>
+        <v>2612983</v>
       </c>
       <c r="B58" s="17">
-        <v>3791190</v>
+        <v>3063975</v>
       </c>
       <c r="C58" s="18">
-        <v>39581462</v>
+        <v>40023506</v>
       </c>
       <c r="D58" s="16">
         <v>3924956</v>
@@ -2670,13 +2670,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
-        <v>2688993</v>
+        <v>2753018</v>
       </c>
       <c r="B59" s="17">
-        <v>3430014</v>
+        <v>2729296</v>
       </c>
       <c r="C59" s="18">
-        <v>39710107</v>
+        <v>41450588</v>
       </c>
       <c r="D59" s="16">
         <v>5633698</v>
@@ -2702,13 +2702,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
-        <v>3570399</v>
+        <v>2748314</v>
       </c>
       <c r="B60" s="17">
-        <v>2806546</v>
+        <v>4396910</v>
       </c>
       <c r="C60" s="18">
-        <v>39818475</v>
+        <v>39656291</v>
       </c>
       <c r="D60" s="16">
         <v>3711978</v>
@@ -2734,13 +2734,13 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
-        <v>2555830</v>
+        <v>2754610</v>
       </c>
       <c r="B61" s="17">
-        <v>3127446</v>
+        <v>2886349</v>
       </c>
       <c r="C61" s="18">
-        <v>38402748</v>
+        <v>39198264</v>
       </c>
       <c r="D61" s="16">
         <v>3935881</v>
@@ -2766,13 +2766,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
-        <v>2559552</v>
+        <v>2279676</v>
       </c>
       <c r="B62" s="17">
-        <v>3560270</v>
+        <v>3971605</v>
       </c>
       <c r="C62" s="18">
-        <v>40189022</v>
+        <v>41129336</v>
       </c>
       <c r="D62" s="16">
         <v>3849216</v>
@@ -2798,13 +2798,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="16">
-        <v>2699919</v>
+        <v>2538967</v>
       </c>
       <c r="B63" s="17">
-        <v>3299591</v>
+        <v>3649388</v>
       </c>
       <c r="C63" s="18">
-        <v>41536844</v>
+        <v>43744282</v>
       </c>
       <c r="D63" s="16">
         <v>3861512</v>
@@ -2830,13 +2830,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="16">
-        <v>2808787</v>
+        <v>3030086</v>
       </c>
       <c r="B64" s="17">
-        <v>3164687</v>
+        <v>3476244</v>
       </c>
       <c r="C64" s="18">
-        <v>40901489</v>
+        <v>40702547</v>
       </c>
       <c r="D64" s="16">
         <v>4194246</v>
@@ -2862,13 +2862,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
-        <v>2580293</v>
+        <v>2624206</v>
       </c>
       <c r="B65" s="17">
-        <v>3626139</v>
+        <v>4119249</v>
       </c>
       <c r="C65" s="18">
-        <v>39853864</v>
+        <v>41622381</v>
       </c>
       <c r="D65" s="16">
         <v>3907864</v>
@@ -2894,13 +2894,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="16">
-        <v>2736437</v>
+        <v>2870997</v>
       </c>
       <c r="B66" s="17">
-        <v>2992135</v>
+        <v>6005599</v>
       </c>
       <c r="C66" s="18">
-        <v>39283914</v>
+        <v>41476014</v>
       </c>
       <c r="D66" s="16">
         <v>3917493</v>
@@ -2926,13 +2926,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="16">
-        <v>2779491</v>
+        <v>2736130</v>
       </c>
       <c r="B67" s="17">
-        <v>2853638</v>
+        <v>4536297</v>
       </c>
       <c r="C67" s="18">
-        <v>41497456</v>
+        <v>42334163</v>
       </c>
       <c r="D67" s="16">
         <v>4496555</v>
@@ -2958,13 +2958,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
-        <v>2471813</v>
+        <v>2498504</v>
       </c>
       <c r="B68" s="17">
-        <v>3374681</v>
+        <v>3046438</v>
       </c>
       <c r="C68" s="18">
-        <v>41487456</v>
+        <v>40635438</v>
       </c>
       <c r="D68" s="16">
         <v>4382891</v>
@@ -2990,13 +2990,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="16">
-        <v>2455462</v>
+        <v>4057936</v>
       </c>
       <c r="B69" s="17">
-        <v>3303738</v>
+        <v>3379079</v>
       </c>
       <c r="C69" s="18">
-        <v>42812407</v>
+        <v>37389985</v>
       </c>
       <c r="D69" s="16">
         <v>3802495</v>
@@ -3022,13 +3022,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="16">
-        <v>2502017</v>
+        <v>2915977</v>
       </c>
       <c r="B70" s="17">
-        <v>3737599</v>
+        <v>3085160</v>
       </c>
       <c r="C70" s="18">
-        <v>41356867</v>
+        <v>43363828</v>
       </c>
       <c r="D70" s="16">
         <v>5709548</v>
@@ -3054,13 +3054,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="16">
-        <v>2592200</v>
+        <v>3948845</v>
       </c>
       <c r="B71" s="17">
-        <v>3303535</v>
+        <v>3084844</v>
       </c>
       <c r="C71" s="18">
-        <v>41866374</v>
+        <v>41190763</v>
       </c>
       <c r="D71" s="16">
         <v>3229340</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
-        <v>2906081</v>
+        <v>2269898</v>
       </c>
       <c r="B72" s="17">
-        <v>3394959</v>
+        <v>3885625</v>
       </c>
       <c r="C72" s="18">
-        <v>40507887</v>
+        <v>43178685</v>
       </c>
       <c r="D72" s="16">
         <v>3465280</v>
@@ -3118,13 +3118,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
-        <v>3021486</v>
+        <v>3210415</v>
       </c>
       <c r="B73" s="17">
-        <v>3462143</v>
+        <v>3030123</v>
       </c>
       <c r="C73" s="18">
-        <v>41174019</v>
+        <v>42255945</v>
       </c>
       <c r="D73" s="16">
         <v>3744107</v>
@@ -3150,13 +3150,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
-        <v>2402481</v>
+        <v>2610150</v>
       </c>
       <c r="B74" s="17">
-        <v>4105906</v>
+        <v>3565483</v>
       </c>
       <c r="C74" s="18">
-        <v>40727437</v>
+        <v>39367281</v>
       </c>
       <c r="D74" s="16">
         <v>4102859</v>
@@ -3182,13 +3182,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="16">
-        <v>2585959</v>
+        <v>3992974</v>
       </c>
       <c r="B75" s="17">
-        <v>3272018</v>
+        <v>3212805</v>
       </c>
       <c r="C75" s="18">
-        <v>39045068</v>
+        <v>43222814</v>
       </c>
       <c r="D75" s="16">
         <v>3779144</v>
@@ -3214,13 +3214,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="16">
-        <v>2775566</v>
+        <v>3184398</v>
       </c>
       <c r="B76" s="17">
-        <v>3292221</v>
+        <v>2991661</v>
       </c>
       <c r="C76" s="18">
-        <v>40870452</v>
+        <v>40690643</v>
       </c>
       <c r="D76" s="16">
         <v>3931788</v>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="16">
-        <v>3944002</v>
+        <v>3335895</v>
       </c>
       <c r="B77" s="17">
-        <v>3302998</v>
+        <v>4138027</v>
       </c>
       <c r="C77" s="18">
-        <v>38463267</v>
+        <v>43264277</v>
       </c>
       <c r="D77" s="16">
         <v>4009046</v>
@@ -3278,13 +3278,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="16">
-        <v>2292281</v>
+        <v>3376282</v>
       </c>
       <c r="B78" s="17">
-        <v>3738266</v>
+        <v>3058993</v>
       </c>
       <c r="C78" s="18">
-        <v>38948996</v>
+        <v>42028320</v>
       </c>
       <c r="D78" s="16">
         <v>3977751</v>
@@ -3310,13 +3310,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="16">
-        <v>2479240</v>
+        <v>3250156</v>
       </c>
       <c r="B79" s="17">
-        <v>3522900</v>
+        <v>3454504</v>
       </c>
       <c r="C79" s="18">
-        <v>36806731</v>
+        <v>38159435</v>
       </c>
       <c r="D79" s="16">
         <v>3954288</v>
@@ -3342,13 +3342,13 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="16">
-        <v>2555126</v>
+        <v>2486838</v>
       </c>
       <c r="B80" s="17">
-        <v>3408607</v>
+        <v>3651222</v>
       </c>
       <c r="C80" s="18">
-        <v>40799213</v>
+        <v>41221428</v>
       </c>
       <c r="D80" s="16">
         <v>4070749</v>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
-        <v>3390811</v>
+        <v>2494949</v>
       </c>
       <c r="B81" s="17">
-        <v>3546566</v>
+        <v>3178824</v>
       </c>
       <c r="C81" s="18">
-        <v>41203685</v>
+        <v>39889586</v>
       </c>
       <c r="D81" s="16">
         <v>4435482</v>
@@ -3406,13 +3406,13 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="16">
-        <v>2527035</v>
+        <v>2893959</v>
       </c>
       <c r="B82" s="17">
-        <v>3504308</v>
+        <v>2616002</v>
       </c>
       <c r="C82" s="18">
-        <v>41742544</v>
+        <v>40522017</v>
       </c>
       <c r="D82" s="16">
         <v>5960228</v>
@@ -3438,13 +3438,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
-        <v>3520178</v>
+        <v>2511968</v>
       </c>
       <c r="B83" s="17">
-        <v>4349363</v>
+        <v>3389524</v>
       </c>
       <c r="C83" s="18">
-        <v>42495822</v>
+        <v>38726812</v>
       </c>
       <c r="D83" s="16">
         <v>5038340</v>
@@ -3470,13 +3470,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
-        <v>2514979</v>
+        <v>3971975</v>
       </c>
       <c r="B84" s="17">
-        <v>3111354</v>
+        <v>4030196</v>
       </c>
       <c r="C84" s="18">
-        <v>41078836</v>
+        <v>42305592</v>
       </c>
       <c r="D84" s="16">
         <v>3278247</v>
@@ -3502,13 +3502,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
-        <v>2740714</v>
+        <v>3105603</v>
       </c>
       <c r="B85" s="17">
-        <v>3383256</v>
+        <v>2872830</v>
       </c>
       <c r="C85" s="18">
-        <v>38689132</v>
+        <v>38996029</v>
       </c>
       <c r="D85" s="16">
         <v>6912004</v>
@@ -3534,13 +3534,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
-        <v>2844675</v>
+        <v>2902459</v>
       </c>
       <c r="B86" s="17">
-        <v>3221611</v>
+        <v>2904348</v>
       </c>
       <c r="C86" s="18">
-        <v>41757451</v>
+        <v>44198313</v>
       </c>
       <c r="D86" s="16">
         <v>5559088</v>
@@ -3566,13 +3566,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
-        <v>2246245</v>
+        <v>2375748</v>
       </c>
       <c r="B87" s="17">
-        <v>3643398</v>
+        <v>3142621</v>
       </c>
       <c r="C87" s="18">
-        <v>42287069</v>
+        <v>40937712</v>
       </c>
       <c r="D87" s="16">
         <v>3654294</v>
@@ -3598,13 +3598,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="16">
-        <v>2486239</v>
+        <v>2398766</v>
       </c>
       <c r="B88" s="17">
-        <v>3321071</v>
+        <v>4374003</v>
       </c>
       <c r="C88" s="18">
-        <v>41210038</v>
+        <v>40917954</v>
       </c>
       <c r="D88" s="16">
         <v>3747051</v>
@@ -3630,13 +3630,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
-        <v>2527497</v>
+        <v>2239380</v>
       </c>
       <c r="B89" s="17">
-        <v>3180390</v>
+        <v>3726924</v>
       </c>
       <c r="C89" s="18">
-        <v>42527934</v>
+        <v>38506206</v>
       </c>
       <c r="D89" s="16">
         <v>3917326</v>
@@ -3662,13 +3662,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
-        <v>2766159</v>
+        <v>2635724</v>
       </c>
       <c r="B90" s="17">
-        <v>3376664</v>
+        <v>3373117</v>
       </c>
       <c r="C90" s="18">
-        <v>39465948</v>
+        <v>36694150</v>
       </c>
       <c r="D90" s="16">
         <v>3471983</v>
@@ -3694,13 +3694,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="16">
-        <v>2538886</v>
+        <v>2789129</v>
       </c>
       <c r="B91" s="17">
-        <v>3217445</v>
+        <v>4033695</v>
       </c>
       <c r="C91" s="18">
-        <v>36947636</v>
+        <v>40266577</v>
       </c>
       <c r="D91" s="16">
         <v>3790977</v>
@@ -3726,13 +3726,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="16">
-        <v>2399148</v>
+        <v>2544967</v>
       </c>
       <c r="B92" s="17">
-        <v>4037333</v>
+        <v>3017457</v>
       </c>
       <c r="C92" s="18">
-        <v>40042194</v>
+        <v>41323297</v>
       </c>
       <c r="D92" s="16">
         <v>5498367</v>
@@ -3758,13 +3758,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="16">
-        <v>2800158</v>
+        <v>2742852</v>
       </c>
       <c r="B93" s="17">
-        <v>4994386</v>
+        <v>3631148</v>
       </c>
       <c r="C93" s="18">
-        <v>36072470</v>
+        <v>40544426</v>
       </c>
       <c r="D93" s="16">
         <v>3835568</v>
@@ -3790,13 +3790,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="16">
-        <v>2645235</v>
+        <v>3075715</v>
       </c>
       <c r="B94" s="17">
-        <v>3896392</v>
+        <v>3961382</v>
       </c>
       <c r="C94" s="18">
-        <v>37149946</v>
+        <v>39217990</v>
       </c>
       <c r="D94" s="16">
         <v>4047156</v>
@@ -3822,13 +3822,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="16">
-        <v>3144353</v>
+        <v>2791314</v>
       </c>
       <c r="B95" s="17">
-        <v>3151372</v>
+        <v>3388598</v>
       </c>
       <c r="C95" s="18">
-        <v>35621111</v>
+        <v>41715385</v>
       </c>
       <c r="D95" s="16">
         <v>3455113</v>
@@ -3854,13 +3854,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
-        <v>2735177</v>
+        <v>3903420</v>
       </c>
       <c r="B96" s="17">
-        <v>4742521</v>
+        <v>3298378</v>
       </c>
       <c r="C96" s="18">
-        <v>38156256</v>
+        <v>40193896</v>
       </c>
       <c r="D96" s="16">
         <v>6547642</v>
@@ -3886,13 +3886,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="16">
-        <v>3785394</v>
+        <v>2765092</v>
       </c>
       <c r="B97" s="17">
-        <v>3068633</v>
+        <v>4578963</v>
       </c>
       <c r="C97" s="18">
-        <v>37673082</v>
+        <v>39282822</v>
       </c>
       <c r="D97" s="16">
         <v>4056823</v>
@@ -3918,13 +3918,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="16">
-        <v>2617736</v>
+        <v>2732241</v>
       </c>
       <c r="B98" s="17">
-        <v>3395274</v>
+        <v>3116362</v>
       </c>
       <c r="C98" s="18">
-        <v>36745140</v>
+        <v>40022900</v>
       </c>
       <c r="D98" s="16">
         <v>4084101</v>
@@ -3950,13 +3950,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="16">
-        <v>2548015</v>
+        <v>2369563</v>
       </c>
       <c r="B99" s="17">
-        <v>3103780</v>
+        <v>3397653</v>
       </c>
       <c r="C99" s="18">
-        <v>37770265</v>
+        <v>39934253</v>
       </c>
       <c r="D99" s="16">
         <v>5973487</v>
@@ -3982,13 +3982,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="16">
-        <v>2554405</v>
+        <v>2620706</v>
       </c>
       <c r="B100" s="17">
-        <v>3268869</v>
+        <v>4204063</v>
       </c>
       <c r="C100" s="18">
-        <v>36945229</v>
+        <v>41182340</v>
       </c>
       <c r="D100" s="16">
         <v>3594573</v>
@@ -4014,13 +4014,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="16">
-        <v>2536590</v>
+        <v>2964199</v>
       </c>
       <c r="B101" s="17">
-        <v>2987710</v>
+        <v>3063123</v>
       </c>
       <c r="C101" s="18">
-        <v>36947062</v>
+        <v>39850848</v>
       </c>
       <c r="D101" s="16">
         <v>4175839</v>
@@ -4046,13 +4046,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="19">
-        <v>2727826</v>
+        <v>3488058</v>
       </c>
       <c r="B102" s="20">
-        <v>2874212</v>
+        <v>4156897</v>
       </c>
       <c r="C102" s="21">
-        <v>36305076</v>
+        <v>37861906</v>
       </c>
       <c r="D102" s="19">
         <v>5700714</v>

</xml_diff>